<commit_message>
Feature/mx 1635 model update biospecimen (#207)
# PR Context
- model update biospecimen
- created [MX-1695] for less confusing wikidata querying

---------

Signed-off-by: erichesse <hessee@rki.de>
</commit_message>
<xml_diff>
--- a/assets/raw-data/biospecimen/test_bioproben.xlsx
+++ b/assets/raw-data/biospecimen/test_bioproben.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20413"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DrebenstedtN\mex-extractors\assets\raw-data\biospecimen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HesseE\mex-extractors\assets\raw-data\biospecimen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4302742E-A624-4FD5-BB67-CD0C85011B95}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EEB91D8-F563-41E7-B90E-CFF69E76466C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -224,12 +224,6 @@
     <t>esterner Testpartner</t>
   </si>
   <si>
-    <t>allgemeiner Testtyp</t>
-  </si>
-  <si>
-    <t>spezieller Testtyp</t>
-  </si>
-  <si>
     <t>Testthema</t>
   </si>
   <si>
@@ -282,6 +276,12 @@
   </si>
   <si>
     <t>test_person@email.de</t>
+  </si>
+  <si>
+    <t>Bioproben</t>
+  </si>
+  <si>
+    <t>Infektionskrankheiten</t>
   </si>
 </sst>
 </file>
@@ -321,7 +321,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -626,9 +626,11 @@
   </sheetPr>
   <dimension ref="A1:B39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="48.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="70.7109375" bestFit="1" customWidth="1"/>
@@ -684,7 +686,7 @@
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -724,7 +726,7 @@
         <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>67</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -732,7 +734,7 @@
         <v>22</v>
       </c>
       <c r="B13" t="s">
-        <v>68</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -740,7 +742,7 @@
         <v>24</v>
       </c>
       <c r="B14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -748,7 +750,7 @@
         <v>26</v>
       </c>
       <c r="B15" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -756,7 +758,7 @@
         <v>26</v>
       </c>
       <c r="B16" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -794,7 +796,7 @@
         <v>29</v>
       </c>
       <c r="B23" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -802,7 +804,7 @@
         <v>31</v>
       </c>
       <c r="B24" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -810,7 +812,7 @@
         <v>33</v>
       </c>
       <c r="B25" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -818,7 +820,7 @@
         <v>35</v>
       </c>
       <c r="B26" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -826,7 +828,7 @@
         <v>37</v>
       </c>
       <c r="B27" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -839,7 +841,7 @@
         <v>39</v>
       </c>
       <c r="B29" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -852,7 +854,7 @@
         <v>41</v>
       </c>
       <c r="B31" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -860,7 +862,7 @@
         <v>43</v>
       </c>
       <c r="B32" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -868,7 +870,7 @@
         <v>45</v>
       </c>
       <c r="B33" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -876,7 +878,7 @@
         <v>47</v>
       </c>
       <c r="B34" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -892,7 +894,7 @@
         <v>51</v>
       </c>
       <c r="B36" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -900,7 +902,7 @@
         <v>53</v>
       </c>
       <c r="B37" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -908,7 +910,7 @@
         <v>55</v>
       </c>
       <c r="B38" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -916,7 +918,7 @@
         <v>57</v>
       </c>
       <c r="B39" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -933,7 +935,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="48.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="71.85546875" bestFit="1" customWidth="1"/>
@@ -989,7 +991,7 @@
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
[mx-1689] wrap up biocspecimen (#271)
# PR Context
- wrap up biospecimen
- depends on mex-assets branch `feature/mx-1689-wrap-up-biospecimen`
</commit_message>
<xml_diff>
--- a/assets/raw-data/biospecimen/test_bioproben.xlsx
+++ b/assets/raw-data/biospecimen/test_bioproben.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20414"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HesseE\mex-extractors\assets\raw-data\biospecimen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EEB91D8-F563-41E7-B90E-CFF69E76466C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7316797D-DDAF-4F51-9CB1-EC4E19DDF1B3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Probe1" sheetId="1" r:id="rId1"/>
@@ -167,9 +167,6 @@
     <t>Zugriffsbeschränkung</t>
   </si>
   <si>
-    <t>Testbeschränkung2</t>
-  </si>
-  <si>
     <t>anonymisiert / pseudonymisiert</t>
   </si>
   <si>
@@ -260,9 +257,6 @@
     <t>Testrechte</t>
   </si>
   <si>
-    <t>Testbeschränkung</t>
-  </si>
-  <si>
     <t>Testdokutitel</t>
   </si>
   <si>
@@ -282,6 +276,12 @@
   </si>
   <si>
     <t>Infektionskrankheiten</t>
+  </si>
+  <si>
+    <t>restriktiv</t>
+  </si>
+  <si>
+    <t>offen</t>
   </si>
 </sst>
 </file>
@@ -626,8 +626,8 @@
   </sheetPr>
   <dimension ref="A1:B39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -654,7 +654,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -662,7 +662,7 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -670,7 +670,7 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -678,7 +678,7 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -686,7 +686,7 @@
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -694,7 +694,7 @@
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -702,7 +702,7 @@
         <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -710,7 +710,7 @@
         <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -718,7 +718,7 @@
         <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -726,7 +726,7 @@
         <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -734,7 +734,7 @@
         <v>22</v>
       </c>
       <c r="B13" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -742,7 +742,7 @@
         <v>24</v>
       </c>
       <c r="B14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -750,7 +750,7 @@
         <v>26</v>
       </c>
       <c r="B15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -758,7 +758,7 @@
         <v>26</v>
       </c>
       <c r="B16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -796,7 +796,7 @@
         <v>29</v>
       </c>
       <c r="B23" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -804,7 +804,7 @@
         <v>31</v>
       </c>
       <c r="B24" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -812,7 +812,7 @@
         <v>33</v>
       </c>
       <c r="B25" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -820,7 +820,7 @@
         <v>35</v>
       </c>
       <c r="B26" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -828,7 +828,7 @@
         <v>37</v>
       </c>
       <c r="B27" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -841,7 +841,7 @@
         <v>39</v>
       </c>
       <c r="B29" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -854,7 +854,7 @@
         <v>41</v>
       </c>
       <c r="B31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -862,7 +862,7 @@
         <v>43</v>
       </c>
       <c r="B32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -870,7 +870,7 @@
         <v>45</v>
       </c>
       <c r="B33" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -878,47 +878,47 @@
         <v>47</v>
       </c>
       <c r="B34" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>48</v>
+      </c>
+      <c r="B35" t="s">
         <v>49</v>
-      </c>
-      <c r="B35" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B36" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B37" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B38" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B39" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -933,7 +933,9 @@
   </sheetPr>
   <dimension ref="A1:B39"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -991,7 +993,7 @@
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1183,47 +1185,47 @@
         <v>47</v>
       </c>
       <c r="B34" t="s">
-        <v>48</v>
+        <v>86</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>48</v>
+      </c>
+      <c r="B35" t="s">
         <v>49</v>
-      </c>
-      <c r="B35" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>50</v>
+      </c>
+      <c r="B36" t="s">
         <v>51</v>
-      </c>
-      <c r="B36" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>52</v>
+      </c>
+      <c r="B37" t="s">
         <v>53</v>
-      </c>
-      <c r="B37" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>54</v>
+      </c>
+      <c r="B38" t="s">
         <v>55</v>
-      </c>
-      <c r="B38" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>56</v>
+      </c>
+      <c r="B39" t="s">
         <v>57</v>
-      </c>
-      <c r="B39" t="s">
-        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>